<commit_message>
Added support for custom organization
</commit_message>
<xml_diff>
--- a/config/organization.xlsx
+++ b/config/organization.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="93">
   <si>
     <t xml:space="preserve">IDENTIFIEUR</t>
   </si>
@@ -206,6 +206,9 @@
   </si>
   <si>
     <t xml:space="preserve">STEPHENSON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-</t>
   </si>
   <si>
     <t xml:space="preserve">BT16</t>
@@ -305,11 +308,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -325,12 +329,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -357,7 +355,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -381,10 +379,6 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -396,14 +390,13 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Normal 2" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -413,10 +406,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="AL1:AM83"/>
+  <dimension ref="AL1:AM88"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AL1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AM13" activeCellId="0" sqref="AM13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AL16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AN38" activeCellId="0" sqref="AN38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -721,192 +714,217 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AL46" s="0" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AL47" s="0" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AL48" s="0" t="s">
-        <v>14</v>
+        <v>62</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AL49" s="0" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AL50" s="0" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AL51" s="0" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AL52" s="0" t="s">
-        <v>16</v>
+        <v>65</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AL53" s="0" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AL54" s="0" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AL55" s="0" t="s">
-        <v>20</v>
+        <v>67</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AL56" s="0" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AL57" s="0" t="s">
-        <v>70</v>
+        <v>16</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AL58" s="0" t="s">
-        <v>71</v>
+        <v>18</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AL59" s="0" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AL60" s="0" t="s">
-        <v>73</v>
+        <v>20</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AL61" s="0" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AL62" s="0" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AL63" s="0" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AL64" s="0" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AL65" s="0" t="s">
-        <v>22</v>
+        <v>74</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AL66" s="0" t="s">
-        <v>23</v>
+        <v>75</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AL67" s="0" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AL68" s="0" t="s">
-        <v>25</v>
+        <v>77</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AL69" s="0" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AL70" s="0" t="s">
-        <v>80</v>
+        <v>22</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AL71" s="0" t="s">
-        <v>81</v>
+        <v>23</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AL72" s="0" t="s">
-        <v>27</v>
+        <v>79</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AL73" s="0" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AL74" s="0" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AL75" s="0" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AL76" s="0" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AL77" s="0" t="s">
-        <v>85</v>
+        <v>27</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AL78" s="0" t="s">
-        <v>86</v>
+        <v>29</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AL79" s="0" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AL80" s="0" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AL81" s="0" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AL82" s="0" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AL83" s="0" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AL84" s="0" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AL85" s="0" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AL86" s="0" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AL87" s="0" t="s">
         <v>91</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AL88" s="0" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>